<commit_message>
add tests on  mainpage
</commit_message>
<xml_diff>
--- a/docs/check- сases.xlsx
+++ b/docs/check- сases.xlsx
@@ -2510,8 +2510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add tests create news
</commit_message>
<xml_diff>
--- a/docs/check- сases.xlsx
+++ b/docs/check- сases.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="242">
   <si>
     <t>№</t>
   </si>
@@ -716,10 +716,6 @@
     <t>Отредактировать объявление. Изменит статус.</t>
   </si>
   <si>
-    <t>News edit-
-Control Panel</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. На экране Control Panel нажать на иконку @id/sort_news_material_button
 2. Нажать на иконку еще раз
 </t>
@@ -792,10 +788,6 @@
     <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку id/edit_news_item_image_view
 2. Изменить Заголовок в объявлении
 3.  Нажать кнопку save</t>
-  </si>
-  <si>
-    <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку @id/add_news_image_view
-3. Нажать кнопку Save</t>
   </si>
   <si>
     <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку @id/add_news_image_view
@@ -1127,6 +1119,25 @@
   </si>
   <si>
     <t>1. На экране выбрать первое объявлеие и нажать на иконку @id/view_news_item_image_view</t>
+  </si>
+  <si>
+    <t>Control Panel</t>
+  </si>
+  <si>
+    <t>News Create, edit</t>
+  </si>
+  <si>
+    <t>Приложение стартовано. Пользователь успешно авторизован. Открыт раздел News - Control Panel-Edit News</t>
+  </si>
+  <si>
+    <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку @id/add_news_image_view
+2. Нажать кнопку Save</t>
+  </si>
+  <si>
+    <t>невозможно</t>
+  </si>
+  <si>
+    <t>Проверка всплывающих сообщений не работает.</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1182,8 +1193,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1379,19 +1396,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color theme="4" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color theme="4" tint="-0.499984740745262"/>
@@ -1400,19 +1404,6 @@
         <color theme="4" tint="-0.499984740745262"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="4" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="medium">
         <color theme="4" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -1580,11 +1571,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1639,20 +1693,14 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1665,9 +1713,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1701,64 +1746,61 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1767,38 +1809,86 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2109,16 +2199,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="27">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="29"/>
+      <c r="B2" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="27"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
@@ -2398,11 +2488,11 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="C29" s="34" t="s">
-        <v>167</v>
+      <c r="B29" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>165</v>
       </c>
       <c r="D29" s="10"/>
     </row>
@@ -2412,7 +2502,7 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D30" s="10"/>
     </row>
@@ -2422,7 +2512,7 @@
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D31" s="10"/>
     </row>
@@ -2432,7 +2522,7 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D32" s="10"/>
     </row>
@@ -2442,7 +2532,7 @@
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D33" s="10"/>
     </row>
@@ -2452,7 +2542,7 @@
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D34" s="10"/>
     </row>
@@ -2462,7 +2552,7 @@
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D35" s="10"/>
     </row>
@@ -2472,7 +2562,7 @@
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D36" s="10"/>
     </row>
@@ -2482,7 +2572,7 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D37" s="10"/>
     </row>
@@ -2492,7 +2582,7 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D38" s="10"/>
     </row>
@@ -2500,11 +2590,11 @@
       <c r="A39" s="7">
         <v>38</v>
       </c>
-      <c r="B39" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>178</v>
+      <c r="B39" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>176</v>
       </c>
       <c r="D39" s="10"/>
     </row>
@@ -2618,13 +2708,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="70" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="66" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.42578125" bestFit="1" customWidth="1"/>
@@ -2636,7 +2726,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
@@ -2649,7 +2739,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>37</v>
@@ -2657,51 +2747,51 @@
       <c r="G1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>155</v>
+      <c r="H1" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>153</v>
       </c>
       <c r="J1" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68">
+      <c r="A2" s="64">
         <v>1</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>154</v>
-      </c>
       <c r="G2" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>159</v>
-      </c>
-      <c r="I2" s="49" t="s">
-        <v>196</v>
-      </c>
-      <c r="J2" s="25"/>
+        <v>155</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="72">
+      <c r="A3" s="68">
         <v>2</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -2710,8 +2800,8 @@
       <c r="D3" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="79" t="s">
-        <v>162</v>
+      <c r="E3" s="77" t="s">
+        <v>160</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>43</v>
@@ -2719,413 +2809,421 @@
       <c r="G3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="J3" s="43"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="69">
+      <c r="H3" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="J3" s="40"/>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="65">
         <v>3</v>
       </c>
-      <c r="B4" s="52"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="19" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I4" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J4" s="45"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="69">
+      <c r="H4" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="J4" s="42" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="65">
         <v>4</v>
       </c>
-      <c r="B5" s="52"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="80"/>
+      <c r="E5" s="78"/>
       <c r="F5" s="19" t="s">
         <v>45</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I5" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J5" s="45"/>
-    </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="69">
+      <c r="H5" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I5" s="75" t="s">
+        <v>240</v>
+      </c>
+      <c r="J5" s="42" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="65">
         <v>5</v>
       </c>
-      <c r="B6" s="52"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="80"/>
+      <c r="E6" s="78"/>
       <c r="F6" s="19" t="s">
         <v>46</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I6" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J6" s="45"/>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="69">
+      <c r="H6" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I6" s="75" t="s">
+        <v>240</v>
+      </c>
+      <c r="J6" s="42" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="65">
         <v>6</v>
       </c>
-      <c r="B7" s="52"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="80"/>
+      <c r="E7" s="78"/>
       <c r="F7" s="19" t="s">
         <v>46</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I7" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J7" s="45"/>
+      <c r="H7" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I7" s="75" t="s">
+        <v>240</v>
+      </c>
+      <c r="J7" s="42" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="74">
+      <c r="A8" s="70">
         <v>7</v>
       </c>
-      <c r="B8" s="53"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="82"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="20" t="s">
         <v>49</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="I8" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="J8" s="47"/>
+      <c r="H8" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="J8" s="44"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="72">
+      <c r="A9" s="68">
         <v>8</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="48" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="E9" s="79" t="s">
-        <v>160</v>
+        <v>198</v>
+      </c>
+      <c r="E9" s="77" t="s">
+        <v>158</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>57</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="H9" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="I9" s="42" t="s">
         <v>196</v>
       </c>
-      <c r="J9" s="43"/>
+      <c r="H9" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="J9" s="40"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="73">
+      <c r="A10" s="69">
         <v>9</v>
       </c>
-      <c r="B10" s="52"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="80"/>
+      <c r="E10" s="78"/>
       <c r="F10" s="15" t="s">
         <v>60</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I10" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J10" s="45"/>
+      <c r="H10" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J10" s="42"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="73">
+      <c r="A11" s="69">
         <v>10</v>
       </c>
-      <c r="B11" s="52"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="80"/>
+      <c r="E11" s="78"/>
       <c r="F11" s="15" t="s">
         <v>61</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I11" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J11" s="45"/>
+      <c r="H11" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="73">
+      <c r="A12" s="69">
         <v>11</v>
       </c>
-      <c r="B12" s="52"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="E12" s="80"/>
+        <v>200</v>
+      </c>
+      <c r="E12" s="78"/>
       <c r="F12" s="19" t="s">
         <v>62</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="H12" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I12" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J12" s="45"/>
+      <c r="H12" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J12" s="42"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="73">
+      <c r="A13" s="69">
         <v>12</v>
       </c>
-      <c r="B13" s="52"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="E13" s="80"/>
+        <v>199</v>
+      </c>
+      <c r="E13" s="78"/>
       <c r="F13" s="19" t="s">
         <v>88</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I13" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J13" s="45"/>
+      <c r="H13" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I13" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J13" s="42"/>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="73">
+      <c r="A14" s="69">
         <v>13</v>
       </c>
-      <c r="B14" s="52"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="80"/>
+      <c r="E14" s="78"/>
       <c r="F14" s="19" t="s">
         <v>83</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I14" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J14" s="45"/>
+      <c r="H14" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I14" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J14" s="42"/>
     </row>
     <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="73">
+      <c r="A15" s="69">
         <v>14</v>
       </c>
-      <c r="B15" s="52"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="80"/>
+      <c r="E15" s="78"/>
       <c r="F15" s="19" t="s">
         <v>70</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I15" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J15" s="45"/>
+      <c r="H15" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I15" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J15" s="42"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="73">
+      <c r="A16" s="69">
         <v>15</v>
       </c>
-      <c r="B16" s="52"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="80"/>
+      <c r="E16" s="78"/>
       <c r="F16" s="19" t="s">
         <v>84</v>
       </c>
       <c r="G16" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I16" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J16" s="45"/>
+      <c r="H16" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I16" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="73">
+      <c r="A17" s="69">
         <v>16</v>
       </c>
-      <c r="B17" s="52"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="80"/>
+      <c r="E17" s="78"/>
       <c r="F17" s="19" t="s">
         <v>87</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I17" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J17" s="45"/>
+      <c r="H17" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I17" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="74">
+      <c r="A18" s="70">
         <v>17</v>
       </c>
-      <c r="B18" s="53"/>
+      <c r="B18" s="50"/>
       <c r="C18" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="82"/>
+      <c r="E18" s="80"/>
       <c r="F18" s="20" t="s">
         <v>85</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="I18" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="J18" s="47"/>
+      <c r="H18" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="I18" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="J18" s="44"/>
     </row>
     <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="72">
+      <c r="A19" s="68">
         <v>18</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="14" t="s">
@@ -3134,8 +3232,8 @@
       <c r="D19" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="79" t="s">
-        <v>160</v>
+      <c r="E19" s="77" t="s">
+        <v>158</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>93</v>
@@ -3143,97 +3241,97 @@
       <c r="G19" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="H19" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="J19" s="43"/>
+      <c r="H19" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="I19" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="73">
+      <c r="A20" s="69">
         <v>19</v>
       </c>
-      <c r="B20" s="52"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="80"/>
+      <c r="E20" s="78"/>
       <c r="F20" s="19" t="s">
         <v>86</v>
       </c>
       <c r="G20" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I20" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J20" s="45"/>
+      <c r="H20" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I20" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="73">
+      <c r="A21" s="69">
         <v>20</v>
       </c>
-      <c r="B21" s="52"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="80"/>
+      <c r="E21" s="78"/>
       <c r="F21" s="19" t="s">
         <v>92</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="H21" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I21" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J21" s="45"/>
+      <c r="H21" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I21" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J21" s="42"/>
     </row>
     <row r="22" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="74">
+      <c r="A22" s="70">
         <v>21</v>
       </c>
-      <c r="B22" s="53"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="82"/>
+      <c r="E22" s="80"/>
       <c r="F22" s="20" t="s">
         <v>91</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="H22" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="I22" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="J22" s="47"/>
+      <c r="H22" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="I22" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="J22" s="44"/>
     </row>
     <row r="23" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="74">
+      <c r="A23" s="70">
         <v>22</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="48" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="14" t="s">
@@ -3242,8 +3340,8 @@
       <c r="D23" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="79" t="s">
-        <v>163</v>
+      <c r="E23" s="77" t="s">
+        <v>161</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>94</v>
@@ -3251,379 +3349,379 @@
       <c r="G23" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H23" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="I23" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="J23" s="43"/>
+      <c r="H23" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="74">
+      <c r="A24" s="70">
         <v>23</v>
       </c>
-      <c r="B24" s="52"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E24" s="78"/>
+      <c r="F24" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="H24" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I24" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J24" s="42"/>
+    </row>
+    <row r="25" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="70">
+        <v>24</v>
+      </c>
+      <c r="B25" s="49"/>
+      <c r="C25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="E25" s="78"/>
+      <c r="F25" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="H25" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="I25" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="J25" s="42"/>
+    </row>
+    <row r="26" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="70">
+        <v>25</v>
+      </c>
+      <c r="B26" s="49"/>
+      <c r="C26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="E24" s="80"/>
-      <c r="F24" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="H24" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I24" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J24" s="45"/>
-    </row>
-    <row r="25" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="74">
-        <v>24</v>
-      </c>
-      <c r="B25" s="52"/>
-      <c r="C25" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="15" t="s">
+      <c r="E26" s="78"/>
+      <c r="F26" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="H26" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="I26" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="J26" s="42"/>
+    </row>
+    <row r="27" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="70">
+        <v>26</v>
+      </c>
+      <c r="B27" s="49"/>
+      <c r="C27" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="E25" s="80"/>
-      <c r="F25" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="G25" s="19" t="s">
+      <c r="E27" s="78"/>
+      <c r="F27" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="H25" s="71" t="s">
-        <v>159</v>
-      </c>
-      <c r="I25" s="71" t="s">
-        <v>196</v>
-      </c>
-      <c r="J25" s="45"/>
-    </row>
-    <row r="26" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="74">
-        <v>25</v>
-      </c>
-      <c r="B26" s="52"/>
-      <c r="C26" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="15" t="s">
+      <c r="G27" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="H27" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="I27" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="J27" s="42"/>
+    </row>
+    <row r="28" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="69">
+        <v>27</v>
+      </c>
+      <c r="B28" s="49"/>
+      <c r="C28" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="E26" s="80"/>
-      <c r="F26" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="H26" s="71" t="s">
-        <v>159</v>
-      </c>
-      <c r="I26" s="71" t="s">
-        <v>196</v>
-      </c>
-      <c r="J26" s="45"/>
-    </row>
-    <row r="27" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="74">
-        <v>26</v>
-      </c>
-      <c r="B27" s="52"/>
-      <c r="C27" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="E27" s="80"/>
-      <c r="F27" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="H27" s="71" t="s">
-        <v>159</v>
-      </c>
-      <c r="I27" s="71" t="s">
-        <v>196</v>
-      </c>
-      <c r="J27" s="45"/>
-    </row>
-    <row r="28" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="73">
-        <v>27</v>
-      </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="E28" s="80"/>
+      <c r="E28" s="78"/>
       <c r="F28" s="19" t="s">
         <v>97</v>
       </c>
       <c r="G28" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="H28" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I28" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J28" s="45"/>
+      <c r="H28" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I28" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="72">
+      <c r="A29" s="68">
         <v>28</v>
       </c>
-      <c r="B29" s="52"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="E29" s="78"/>
+      <c r="F29" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="G29" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="E29" s="80"/>
-      <c r="F29" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="45"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="42"/>
     </row>
     <row r="30" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="72">
+      <c r="A30" s="68">
         <v>29</v>
       </c>
-      <c r="B30" s="52"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="E30" s="78"/>
+      <c r="F30" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="G30" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="E30" s="80"/>
-      <c r="F30" s="19" t="s">
+      <c r="H30" s="71" t="s">
         <v>223</v>
       </c>
-      <c r="G30" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="H30" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="I30" s="75" t="s">
-        <v>196</v>
-      </c>
-      <c r="J30" s="45"/>
+      <c r="I30" s="71" t="s">
+        <v>194</v>
+      </c>
+      <c r="J30" s="42"/>
     </row>
     <row r="31" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="72">
+      <c r="A31" s="68">
         <v>30</v>
       </c>
-      <c r="B31" s="52"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="80"/>
+      <c r="E31" s="78"/>
       <c r="F31" s="19" t="s">
         <v>99</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="H31" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I31" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J31" s="45"/>
+      <c r="H31" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I31" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J31" s="42"/>
     </row>
     <row r="32" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="72">
+      <c r="A32" s="68">
         <v>31</v>
       </c>
-      <c r="B32" s="52"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="80"/>
+      <c r="E32" s="78"/>
       <c r="F32" s="19" t="s">
         <v>102</v>
       </c>
       <c r="G32" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H32" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I32" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J32" s="45"/>
+      <c r="H32" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I32" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J32" s="42"/>
     </row>
     <row r="33" spans="1:10" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="72">
+      <c r="A33" s="68">
         <v>32</v>
       </c>
-      <c r="B33" s="52"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="80"/>
+      <c r="E33" s="78"/>
       <c r="F33" s="19" t="s">
         <v>105</v>
       </c>
       <c r="G33" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="H33" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I33" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J33" s="45"/>
+      <c r="H33" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I33" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J33" s="42"/>
     </row>
     <row r="34" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="72">
+      <c r="A34" s="68">
         <v>33</v>
       </c>
-      <c r="B34" s="52"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="80"/>
+      <c r="E34" s="78"/>
       <c r="F34" s="19" t="s">
         <v>109</v>
       </c>
       <c r="G34" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="H34" s="44" t="s">
-        <v>221</v>
-      </c>
-      <c r="I34" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J34" s="45"/>
+      <c r="H34" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="I34" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J34" s="42"/>
     </row>
     <row r="35" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="72">
+      <c r="A35" s="68">
         <v>34</v>
       </c>
-      <c r="B35" s="52"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="E35" s="80"/>
+        <v>217</v>
+      </c>
+      <c r="E35" s="78"/>
       <c r="F35" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G35" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="H35" s="44" t="s">
-        <v>221</v>
-      </c>
-      <c r="I35" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J35" s="45"/>
+      <c r="H35" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="I35" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J35" s="42"/>
     </row>
     <row r="36" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="72">
+      <c r="A36" s="68">
         <v>35</v>
       </c>
-      <c r="B36" s="52"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="80"/>
+      <c r="E36" s="78"/>
       <c r="F36" s="19" t="s">
         <v>111</v>
       </c>
       <c r="G36" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="H36" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I36" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J36" s="45"/>
+      <c r="H36" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I36" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J36" s="42"/>
     </row>
     <row r="37" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="72">
+      <c r="A37" s="68">
         <v>36</v>
       </c>
-      <c r="B37" s="53"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D37" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="82"/>
+      <c r="E37" s="80"/>
       <c r="F37" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="H37" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="I37" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="J37" s="47"/>
+      <c r="H37" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="I37" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="J37" s="44"/>
     </row>
     <row r="38" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="72">
+      <c r="A38" s="68">
         <v>37</v>
       </c>
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="48" t="s">
         <v>21</v>
       </c>
       <c r="C38" s="14" t="s">
@@ -3632,8 +3730,8 @@
       <c r="D38" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E38" s="79" t="s">
-        <v>164</v>
+      <c r="E38" s="77" t="s">
+        <v>162</v>
       </c>
       <c r="F38" s="18" t="s">
         <v>117</v>
@@ -3641,98 +3739,98 @@
       <c r="G38" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="H38" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="I38" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J38" s="43"/>
+      <c r="H38" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="I38" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="72">
+      <c r="A39" s="68">
         <v>38</v>
       </c>
-      <c r="B39" s="52"/>
+      <c r="B39" s="49"/>
       <c r="C39" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D39" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="E39" s="78"/>
+      <c r="F39" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="G39" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="E39" s="80"/>
-      <c r="F39" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="H39" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I39" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J39" s="45"/>
+      <c r="H39" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I39" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J39" s="42"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="72">
+      <c r="A40" s="68">
         <v>39</v>
       </c>
-      <c r="B40" s="53"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E40" s="82"/>
+      <c r="E40" s="80"/>
       <c r="F40" s="20" t="s">
         <v>119</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="H40" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="I40" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="J40" s="47"/>
+      <c r="H40" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="I40" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="J40" s="44"/>
     </row>
     <row r="41" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="72">
-        <v>40</v>
-      </c>
-      <c r="B41" s="53"/>
+      <c r="A41" s="68">
+        <v>40</v>
+      </c>
+      <c r="B41" s="50"/>
       <c r="C41" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D41" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="78"/>
+      <c r="E41" s="73"/>
       <c r="F41" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="H41" s="77" t="s">
-        <v>159</v>
-      </c>
-      <c r="I41" s="77" t="s">
-        <v>196</v>
-      </c>
-      <c r="J41" s="47"/>
-    </row>
-    <row r="42" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="72">
+      <c r="H41" s="72" t="s">
+        <v>157</v>
+      </c>
+      <c r="I41" s="72" t="s">
+        <v>194</v>
+      </c>
+      <c r="J41" s="44"/>
+    </row>
+    <row r="42" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="82">
         <v>41</v>
       </c>
-      <c r="B42" s="54" t="s">
-        <v>130</v>
+      <c r="B42" s="83" t="s">
+        <v>236</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>40</v>
@@ -3740,341 +3838,347 @@
       <c r="D42" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="79" t="s">
-        <v>165</v>
+      <c r="E42" s="77" t="s">
+        <v>163</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G42" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="H42" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="I42" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J42" s="43"/>
-    </row>
-    <row r="43" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="72">
+      <c r="H42" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="I42" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="J42" s="40"/>
+    </row>
+    <row r="43" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="84">
         <v>42</v>
       </c>
-      <c r="B43" s="52"/>
+      <c r="B43" s="85"/>
       <c r="C43" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E43" s="80"/>
+      <c r="E43" s="78"/>
       <c r="F43" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="H43" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I43" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J43" s="45"/>
-    </row>
-    <row r="44" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="72">
+        <v>227</v>
+      </c>
+      <c r="H43" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="I43" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="J43" s="42"/>
+    </row>
+    <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="84">
         <v>43</v>
       </c>
-      <c r="B44" s="52"/>
+      <c r="B44" s="85"/>
       <c r="C44" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E44" s="80"/>
+      <c r="E44" s="78"/>
       <c r="F44" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="H44" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="I44" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="J44" s="42"/>
+    </row>
+    <row r="45" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="84">
+        <v>44</v>
+      </c>
+      <c r="B45" s="85"/>
+      <c r="C45" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="78"/>
+      <c r="F45" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="G45" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="G44" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="H44" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I44" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J44" s="45"/>
-    </row>
-    <row r="45" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="72">
-        <v>44</v>
-      </c>
-      <c r="B45" s="52"/>
-      <c r="C45" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="E45" s="80"/>
-      <c r="F45" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="G45" s="19" t="s">
+      <c r="H45" s="75" t="s">
         <v>234</v>
       </c>
-      <c r="H45" s="76" t="s">
-        <v>236</v>
-      </c>
-      <c r="I45" s="76" t="s">
-        <v>196</v>
-      </c>
-      <c r="J45" s="45"/>
-    </row>
-    <row r="46" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="72">
+      <c r="I45" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="J45" s="42"/>
+    </row>
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="84">
         <v>45</v>
       </c>
-      <c r="B46" s="53"/>
-      <c r="C46" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D46" s="16" t="s">
+      <c r="B46" s="85"/>
+      <c r="C46" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E46" s="80"/>
-      <c r="F46" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="G46" s="20" t="s">
+      <c r="E46" s="78"/>
+      <c r="F46" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G46" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H46" s="77" t="s">
-        <v>159</v>
-      </c>
-      <c r="I46" s="77" t="s">
-        <v>196</v>
-      </c>
-      <c r="J46" s="47"/>
+      <c r="H46" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="I46" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="J46" s="42"/>
     </row>
     <row r="47" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="72">
+      <c r="A47" s="86">
         <v>46</v>
       </c>
-      <c r="B47" s="52"/>
-      <c r="C47" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47" s="15" t="s">
+      <c r="B47" s="87"/>
+      <c r="C47" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="16" t="s">
         <v>27</v>
       </c>
       <c r="E47" s="80"/>
-      <c r="F47" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="G47" s="19" t="s">
+      <c r="F47" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="G47" s="20" t="s">
         <v>124</v>
       </c>
       <c r="H47" s="76" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I47" s="76" t="s">
-        <v>196</v>
-      </c>
-      <c r="J47" s="45"/>
+        <v>194</v>
+      </c>
+      <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="68">
+      <c r="A48" s="86">
         <v>47</v>
       </c>
-      <c r="B48" s="52"/>
-      <c r="C48" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" s="15" t="s">
+      <c r="B48" s="83" t="s">
+        <v>237</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="80"/>
-      <c r="F48" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="G48" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="H48" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I48" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J48" s="45"/>
-    </row>
-    <row r="49" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="68">
+      <c r="E48" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H48" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="I48" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="J48" s="40"/>
+    </row>
+    <row r="49" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="94">
         <v>48</v>
       </c>
-      <c r="B49" s="52"/>
+      <c r="B49" s="85"/>
       <c r="C49" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D49" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E49" s="78"/>
+      <c r="F49" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="G49" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="E49" s="80"/>
-      <c r="F49" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G49" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="H49" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I49" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J49" s="45"/>
-    </row>
-    <row r="50" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="68">
+      <c r="H49" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="I49" s="75" t="s">
+        <v>240</v>
+      </c>
+      <c r="J49" s="42" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="92">
         <v>49</v>
       </c>
-      <c r="B50" s="52"/>
+      <c r="B50" s="85"/>
       <c r="C50" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="E50" s="80"/>
+      <c r="E50" s="78"/>
       <c r="F50" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="H50" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I50" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J50" s="45"/>
-    </row>
-    <row r="51" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="68">
+        <v>131</v>
+      </c>
+      <c r="H50" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="I50" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="J50" s="42"/>
+    </row>
+    <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="92">
         <v>50</v>
       </c>
-      <c r="B51" s="52"/>
+      <c r="B51" s="85"/>
       <c r="C51" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E51" s="80"/>
+      <c r="E51" s="78"/>
       <c r="F51" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G51" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H51" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="I51" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="J51" s="42"/>
+    </row>
+    <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="92">
+        <v>51</v>
+      </c>
+      <c r="B52" s="85"/>
+      <c r="C52" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="H51" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I51" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J51" s="45"/>
-    </row>
-    <row r="52" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="68">
-        <v>51</v>
-      </c>
-      <c r="B52" s="52"/>
-      <c r="C52" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D52" s="15" t="s">
+      <c r="E52" s="78"/>
+      <c r="F52" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="G52" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="E52" s="80"/>
-      <c r="F52" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="G52" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="H52" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I52" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J52" s="45"/>
-    </row>
-    <row r="53" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="68">
+      <c r="H52" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="I52" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="J52" s="42"/>
+    </row>
+    <row r="53" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53" s="92">
         <v>52</v>
       </c>
-      <c r="B53" s="52"/>
+      <c r="B53" s="85"/>
       <c r="C53" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="E53" s="80"/>
+      <c r="E53" s="78"/>
       <c r="F53" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G53" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="H53" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="I53" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="J53" s="42"/>
+    </row>
+    <row r="54" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="93">
+        <v>53</v>
+      </c>
+      <c r="B54" s="87"/>
+      <c r="C54" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" s="80"/>
+      <c r="F54" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="H53" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I53" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J53" s="45"/>
-    </row>
-    <row r="54" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="68">
-        <v>53</v>
-      </c>
-      <c r="B54" s="52"/>
-      <c r="C54" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" s="80"/>
-      <c r="F54" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G54" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="H54" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="I54" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J54" s="45"/>
+      <c r="H54" s="76" t="s">
+        <v>157</v>
+      </c>
+      <c r="I54" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="J54" s="44"/>
     </row>
     <row r="55" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="68">
+      <c r="A55" s="81">
         <v>54</v>
       </c>
-      <c r="B55" s="55" t="s">
-        <v>199</v>
+      <c r="B55" s="51" t="s">
+        <v>197</v>
       </c>
       <c r="C55" s="21" t="s">
         <v>40</v>
@@ -4082,325 +4186,326 @@
       <c r="D55" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E55" s="32"/>
-      <c r="F55" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="G55" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="H55" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="I55" s="49" t="s">
-        <v>196</v>
-      </c>
-      <c r="J55" s="26"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="G55" s="88" t="s">
+        <v>149</v>
+      </c>
+      <c r="H55" s="89" t="s">
+        <v>157</v>
+      </c>
+      <c r="I55" s="90" t="s">
+        <v>194</v>
+      </c>
+      <c r="J55" s="91"/>
     </row>
     <row r="56" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="68">
+      <c r="A56" s="64">
         <v>55</v>
       </c>
-      <c r="B56" s="56" t="s">
+      <c r="B56" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="E56" s="77" t="s">
+        <v>178</v>
+      </c>
+      <c r="F56" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="G56" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="H56" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="I56" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="J56" s="47"/>
+    </row>
+    <row r="57" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="64">
+        <v>56</v>
+      </c>
+      <c r="B57" s="53"/>
+      <c r="C57" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="E57" s="78"/>
+      <c r="F57" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="G57" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="H57" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="I57" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="J57" s="10"/>
+    </row>
+    <row r="58" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="64">
+        <v>57</v>
+      </c>
+      <c r="B58" s="53"/>
+      <c r="C58" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="E58" s="78"/>
+      <c r="F58" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="G58" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="H58" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="I58" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="J58" s="10"/>
+    </row>
+    <row r="59" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="64">
+        <v>58</v>
+      </c>
+      <c r="B59" s="53"/>
+      <c r="C59" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="E59" s="78"/>
+      <c r="F59" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="G59" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="H59" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="I59" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="J59" s="10"/>
+    </row>
+    <row r="60" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="64">
+        <v>59</v>
+      </c>
+      <c r="B60" s="53"/>
+      <c r="C60" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="E60" s="78"/>
+      <c r="F60" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="G60" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="H60" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="I60" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="J60" s="10"/>
+    </row>
+    <row r="61" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="64">
+        <v>60</v>
+      </c>
+      <c r="B61" s="53"/>
+      <c r="C61" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="E61" s="78"/>
+      <c r="F61" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="G61" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="H61" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="I61" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="J61" s="10"/>
+    </row>
+    <row r="62" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="64">
+        <v>61</v>
+      </c>
+      <c r="B62" s="53"/>
+      <c r="C62" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="E62" s="78"/>
+      <c r="F62" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="G62" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="H62" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="I62" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="J62" s="10"/>
+    </row>
+    <row r="63" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="64">
+        <v>62</v>
+      </c>
+      <c r="B63" s="53"/>
+      <c r="C63" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="C56" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D56" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="E56" s="79" t="s">
-        <v>180</v>
-      </c>
-      <c r="F56" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="G56" s="40" t="s">
-        <v>182</v>
-      </c>
-      <c r="H56" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="I56" s="41" t="s">
-        <v>197</v>
-      </c>
-      <c r="J56" s="50"/>
-    </row>
-    <row r="57" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="68">
-        <v>56</v>
-      </c>
-      <c r="B57" s="57"/>
-      <c r="C57" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D57" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="E57" s="80"/>
-      <c r="F57" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="G57" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="H57" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="I57" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="J57" s="10"/>
-    </row>
-    <row r="58" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="68">
-        <v>57</v>
-      </c>
-      <c r="B58" s="57"/>
-      <c r="C58" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D58" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="E58" s="80"/>
-      <c r="F58" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="G58" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="H58" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="I58" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="J58" s="10"/>
-    </row>
-    <row r="59" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="68">
-        <v>58</v>
-      </c>
-      <c r="B59" s="57"/>
-      <c r="C59" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D59" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="E59" s="80"/>
-      <c r="F59" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="G59" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="H59" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="I59" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="J59" s="10"/>
-    </row>
-    <row r="60" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="68">
-        <v>59</v>
-      </c>
-      <c r="B60" s="57"/>
-      <c r="C60" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D60" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="E60" s="80"/>
-      <c r="F60" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="G60" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="H60" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="I60" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="J60" s="10"/>
-    </row>
-    <row r="61" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="68">
-        <v>60</v>
-      </c>
-      <c r="B61" s="57"/>
-      <c r="C61" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D61" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="E61" s="80"/>
-      <c r="F61" s="37" t="s">
+      <c r="E63" s="78"/>
+      <c r="F63" s="34" t="s">
         <v>191</v>
       </c>
-      <c r="G61" s="37" t="s">
+      <c r="G63" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="H61" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="I61" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="J61" s="10"/>
-    </row>
-    <row r="62" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="68">
-        <v>61</v>
-      </c>
-      <c r="B62" s="57"/>
-      <c r="C62" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D62" s="34" t="s">
+      <c r="H63" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="I63" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="J63" s="10"/>
+    </row>
+    <row r="64" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="53"/>
+      <c r="C64" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="E62" s="80"/>
-      <c r="F62" s="37" t="s">
+      <c r="E64" s="78"/>
+      <c r="F64" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="G64" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="H64" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="I64" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="J64" s="10"/>
+    </row>
+    <row r="65" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="64">
+        <v>64</v>
+      </c>
+      <c r="B65" s="55"/>
+      <c r="C65" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" s="57" t="s">
+        <v>174</v>
+      </c>
+      <c r="E65" s="79"/>
+      <c r="F65" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="G65" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="H65" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="I65" s="59" t="s">
+        <v>195</v>
+      </c>
+      <c r="J65" s="60"/>
+    </row>
+    <row r="66" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="64">
+        <v>65</v>
+      </c>
+      <c r="B66" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="C66" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="62" t="s">
+        <v>176</v>
+      </c>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="G66" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="G62" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="H62" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="I62" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="J62" s="10"/>
-    </row>
-    <row r="63" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="68">
-        <v>62</v>
-      </c>
-      <c r="B63" s="57"/>
-      <c r="C63" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D63" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="E63" s="80"/>
-      <c r="F63" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="G63" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="H63" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="I63" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="J63" s="10"/>
-    </row>
-    <row r="64" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="68">
-        <v>63</v>
-      </c>
-      <c r="B64" s="57"/>
-      <c r="C64" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D64" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="E64" s="80"/>
-      <c r="F64" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="G64" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="H64" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="I64" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="J64" s="10"/>
-    </row>
-    <row r="65" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="68">
-        <v>64</v>
-      </c>
-      <c r="B65" s="59"/>
-      <c r="C65" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="D65" s="61" t="s">
-        <v>176</v>
-      </c>
-      <c r="E65" s="81"/>
-      <c r="F65" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="G65" s="62" t="s">
-        <v>194</v>
-      </c>
-      <c r="H65" s="63" t="s">
-        <v>159</v>
-      </c>
-      <c r="I65" s="63" t="s">
-        <v>197</v>
-      </c>
-      <c r="J65" s="64"/>
-    </row>
-    <row r="66" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="68">
-        <v>65</v>
-      </c>
-      <c r="B66" s="65" t="s">
-        <v>177</v>
-      </c>
-      <c r="C66" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="D66" s="66" t="s">
-        <v>178</v>
-      </c>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48" t="s">
-        <v>193</v>
-      </c>
-      <c r="G66" s="48" t="s">
+      <c r="H66" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="I66" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="H66" s="49" t="s">
-        <v>159</v>
-      </c>
-      <c r="I66" s="49" t="s">
-        <v>197</v>
-      </c>
-      <c r="J66" s="67"/>
+      <c r="J66" s="63"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="68"/>
+      <c r="A67" s="64"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E42:E54"/>
+  <mergeCells count="8">
     <mergeCell ref="E56:E65"/>
     <mergeCell ref="E3:E8"/>
     <mergeCell ref="E9:E18"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="E23:E37"/>
     <mergeCell ref="E38:E40"/>
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="E48:E54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
create unit  tests finished
</commit_message>
<xml_diff>
--- a/docs/check- сases.xlsx
+++ b/docs/check- сases.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="236">
   <si>
     <t>№</t>
   </si>
@@ -704,15 +704,6 @@
     <t>1. Объявление раскроется, описание отображается.</t>
   </si>
   <si>
-    <t>Отредактировать в объявлении Title</t>
-  </si>
-  <si>
-    <t>Отредактировать в объявлении Date</t>
-  </si>
-  <si>
-    <t>Отредактировать в объявлении Description</t>
-  </si>
-  <si>
     <t>Отредактировать объявление. Изменит статус.</t>
   </si>
   <si>
@@ -722,31 +713,8 @@
   </si>
   <si>
     <t>1. Откроется экран редактирвоания объявления
-2. Заголовок изменен
-3. В объявлении изменен заголовок</t>
-  </si>
-  <si>
-    <t>1. Откроется экран редактирвоания объявления
-2. Опсание изменено
-3. В объявлении изменено описание</t>
-  </si>
-  <si>
-    <t>1. Откроется экран редактирвоания объявления
 2. Свитчер переключен
 3. В объявлении изменен статус</t>
-  </si>
-  <si>
-    <t>1. Откроется экран редактирвоания объявления
-2. Дата изменена
-3. В объявлении изменена дата</t>
-  </si>
-  <si>
-    <t>Отредактировать в объявлении Time</t>
-  </si>
-  <si>
-    <t>1. Откроется экран редактирвоания объявления
-2. Время изменена
-3. В объявлении изменено время</t>
   </si>
   <si>
     <t>1. Откроется экран создания объявления
@@ -767,26 +735,6 @@
   <si>
     <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку id/edit_news_item_image_view
 2. Перещелкнуть свитчер Active
-3.  Нажать кнопку save</t>
-  </si>
-  <si>
-    <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку id/edit_news_item_image_view
-2. Изменить Описаниев объявлении
-3.  Нажать кнопку save</t>
-  </si>
-  <si>
-    <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку id/edit_news_item_image_view
-2. Изменить время  в объявлении
-3.  Нажать кнопку save</t>
-  </si>
-  <si>
-    <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку id/edit_news_item_image_view
-2. Изменить даты  в объявлении
-3.  Нажать кнопку save</t>
-  </si>
-  <si>
-    <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку id/edit_news_item_image_view
-2. Изменить Заголовок в объявлении
 3.  Нажать кнопку save</t>
   </si>
   <si>
@@ -1138,6 +1086,32 @@
   </si>
   <si>
     <t>Проверка всплывающих сообщений не работает.</t>
+  </si>
+  <si>
+    <t>Отредактировать в объявлении Title, Date,Time, Description</t>
+  </si>
+  <si>
+    <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку id/edit_news_item_image_view
+2. Изменить поля
+3.  Нажать кнопку save</t>
+  </si>
+  <si>
+    <t>1. Откроется экран редактирвоания объявления
+2. Поля изменены
+3. В объявлении изменены поля Title, Date,Time, Description</t>
+  </si>
+  <si>
+    <t>Отменить редактирование</t>
+  </si>
+  <si>
+    <t>1. На экране Control Panel выбрать первое объявлеие и нажать на иконку id/edit_news_item_image_view
+2. Изменить поля
+3.  Нажать кнопку cancel и подвердить</t>
+  </si>
+  <si>
+    <t>1. Откроется экран редактирвоания объявления
+2. Поля изменены
+3. В объявлении  поля отстались неизмененными</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1572,17 +1546,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color theme="4" tint="-0.499984740745262"/>
       </left>
@@ -1638,7 +1601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1800,9 +1763,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1836,6 +1796,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1847,48 +1843,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2203,10 +2157,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D2" s="27"/>
     </row>
@@ -2489,10 +2443,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D29" s="10"/>
     </row>
@@ -2502,7 +2456,7 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="9" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D30" s="10"/>
     </row>
@@ -2512,7 +2466,7 @@
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="9" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D31" s="10"/>
     </row>
@@ -2522,7 +2476,7 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="9" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D32" s="10"/>
     </row>
@@ -2532,7 +2486,7 @@
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="9" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D33" s="10"/>
     </row>
@@ -2542,7 +2496,7 @@
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D34" s="10"/>
     </row>
@@ -2552,7 +2506,7 @@
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="9" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="D35" s="10"/>
     </row>
@@ -2562,7 +2516,7 @@
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="9" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="D36" s="10"/>
     </row>
@@ -2572,7 +2526,7 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="9" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D37" s="10"/>
     </row>
@@ -2582,7 +2536,7 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="9" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D38" s="10"/>
     </row>
@@ -2591,10 +2545,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D39" s="10"/>
     </row>
@@ -2706,15 +2660,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="66" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.42578125" bestFit="1" customWidth="1"/>
@@ -2722,7 +2676,7 @@
     <col min="6" max="6" width="62.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="39.140625" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2739,7 +2693,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>37</v>
@@ -2748,10 +2702,10 @@
         <v>38</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="J1" s="22" t="s">
         <v>2</v>
@@ -2762,33 +2716,33 @@
         <v>1</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I2" s="46" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="68">
+      <c r="A3" s="67">
         <v>2</v>
       </c>
       <c r="B3" s="48" t="s">
@@ -2800,8 +2754,8 @@
       <c r="D3" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="77" t="s">
-        <v>160</v>
+      <c r="E3" s="88" t="s">
+        <v>148</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>43</v>
@@ -2810,15 +2764,15 @@
         <v>42</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="65">
+      <c r="A4" s="87">
         <v>3</v>
       </c>
       <c r="B4" s="49"/>
@@ -2828,7 +2782,7 @@
       <c r="D4" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="78"/>
+      <c r="E4" s="89"/>
       <c r="F4" s="19" t="s">
         <v>44</v>
       </c>
@@ -2836,17 +2790,17 @@
         <v>47</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I4" s="41" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="J4" s="42" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="65">
+      <c r="A5" s="87">
         <v>4</v>
       </c>
       <c r="B5" s="49"/>
@@ -2856,7 +2810,7 @@
       <c r="D5" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="78"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="19" t="s">
         <v>45</v>
       </c>
@@ -2864,17 +2818,17 @@
         <v>47</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="I5" s="75" t="s">
-        <v>240</v>
+        <v>145</v>
+      </c>
+      <c r="I5" s="74" t="s">
+        <v>228</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="65">
+      <c r="A6" s="87">
         <v>5</v>
       </c>
       <c r="B6" s="49"/>
@@ -2884,7 +2838,7 @@
       <c r="D6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="78"/>
+      <c r="E6" s="89"/>
       <c r="F6" s="19" t="s">
         <v>46</v>
       </c>
@@ -2892,17 +2846,17 @@
         <v>48</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="I6" s="75" t="s">
-        <v>240</v>
+        <v>145</v>
+      </c>
+      <c r="I6" s="74" t="s">
+        <v>228</v>
       </c>
       <c r="J6" s="42" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="65">
+      <c r="A7" s="87">
         <v>6</v>
       </c>
       <c r="B7" s="49"/>
@@ -2912,7 +2866,7 @@
       <c r="D7" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="78"/>
+      <c r="E7" s="89"/>
       <c r="F7" s="19" t="s">
         <v>46</v>
       </c>
@@ -2920,17 +2874,17 @@
         <v>48</v>
       </c>
       <c r="H7" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="I7" s="75" t="s">
-        <v>240</v>
+        <v>145</v>
+      </c>
+      <c r="I7" s="74" t="s">
+        <v>228</v>
       </c>
       <c r="J7" s="42" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="70">
+      <c r="A8" s="69">
         <v>7</v>
       </c>
       <c r="B8" s="50"/>
@@ -2940,7 +2894,7 @@
       <c r="D8" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="80"/>
+      <c r="E8" s="91"/>
       <c r="F8" s="20" t="s">
         <v>49</v>
       </c>
@@ -2948,15 +2902,15 @@
         <v>50</v>
       </c>
       <c r="H8" s="43" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I8" s="43" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J8" s="44"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="68">
+      <c r="A9" s="67">
         <v>8</v>
       </c>
       <c r="B9" s="48" t="s">
@@ -2966,27 +2920,27 @@
         <v>40</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="E9" s="77" t="s">
-        <v>158</v>
+        <v>186</v>
+      </c>
+      <c r="E9" s="88" t="s">
+        <v>146</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>57</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="H9" s="39" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I9" s="39" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J9" s="40"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="69">
+      <c r="A10" s="68">
         <v>9</v>
       </c>
       <c r="B10" s="49"/>
@@ -2996,7 +2950,7 @@
       <c r="D10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="78"/>
+      <c r="E10" s="89"/>
       <c r="F10" s="15" t="s">
         <v>60</v>
       </c>
@@ -3004,15 +2958,15 @@
         <v>58</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I10" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J10" s="42"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="69">
+      <c r="A11" s="68">
         <v>10</v>
       </c>
       <c r="B11" s="49"/>
@@ -3022,7 +2976,7 @@
       <c r="D11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="78"/>
+      <c r="E11" s="89"/>
       <c r="F11" s="15" t="s">
         <v>61</v>
       </c>
@@ -3030,15 +2984,15 @@
         <v>59</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I11" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="69">
+      <c r="A12" s="68">
         <v>11</v>
       </c>
       <c r="B12" s="49"/>
@@ -3046,9 +3000,9 @@
         <v>40</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="E12" s="78"/>
+        <v>188</v>
+      </c>
+      <c r="E12" s="89"/>
       <c r="F12" s="19" t="s">
         <v>62</v>
       </c>
@@ -3056,15 +3010,15 @@
         <v>69</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J12" s="42"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="69">
+      <c r="A13" s="68">
         <v>12</v>
       </c>
       <c r="B13" s="49"/>
@@ -3072,9 +3026,9 @@
         <v>40</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="E13" s="78"/>
+        <v>187</v>
+      </c>
+      <c r="E13" s="89"/>
       <c r="F13" s="19" t="s">
         <v>88</v>
       </c>
@@ -3082,15 +3036,15 @@
         <v>63</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I13" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J13" s="42"/>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="69">
+      <c r="A14" s="68">
         <v>13</v>
       </c>
       <c r="B14" s="49"/>
@@ -3100,7 +3054,7 @@
       <c r="D14" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="78"/>
+      <c r="E14" s="89"/>
       <c r="F14" s="19" t="s">
         <v>83</v>
       </c>
@@ -3108,15 +3062,15 @@
         <v>73</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I14" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J14" s="42"/>
     </row>
     <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="69">
+      <c r="A15" s="68">
         <v>14</v>
       </c>
       <c r="B15" s="49"/>
@@ -3126,7 +3080,7 @@
       <c r="D15" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="78"/>
+      <c r="E15" s="89"/>
       <c r="F15" s="19" t="s">
         <v>70</v>
       </c>
@@ -3134,15 +3088,15 @@
         <v>71</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J15" s="42"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="69">
+      <c r="A16" s="68">
         <v>15</v>
       </c>
       <c r="B16" s="49"/>
@@ -3152,7 +3106,7 @@
       <c r="D16" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="78"/>
+      <c r="E16" s="89"/>
       <c r="F16" s="19" t="s">
         <v>84</v>
       </c>
@@ -3160,15 +3114,15 @@
         <v>89</v>
       </c>
       <c r="H16" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I16" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="69">
+      <c r="A17" s="68">
         <v>16</v>
       </c>
       <c r="B17" s="49"/>
@@ -3178,7 +3132,7 @@
       <c r="D17" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="78"/>
+      <c r="E17" s="89"/>
       <c r="F17" s="19" t="s">
         <v>87</v>
       </c>
@@ -3186,15 +3140,15 @@
         <v>72</v>
       </c>
       <c r="H17" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I17" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="70">
+      <c r="A18" s="69">
         <v>17</v>
       </c>
       <c r="B18" s="50"/>
@@ -3204,7 +3158,7 @@
       <c r="D18" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="80"/>
+      <c r="E18" s="91"/>
       <c r="F18" s="20" t="s">
         <v>85</v>
       </c>
@@ -3212,15 +3166,15 @@
         <v>74</v>
       </c>
       <c r="H18" s="43" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I18" s="43" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J18" s="44"/>
     </row>
     <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="68">
+      <c r="A19" s="67">
         <v>18</v>
       </c>
       <c r="B19" s="48" t="s">
@@ -3232,8 +3186,8 @@
       <c r="D19" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="77" t="s">
-        <v>158</v>
+      <c r="E19" s="88" t="s">
+        <v>146</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>93</v>
@@ -3242,15 +3196,15 @@
         <v>79</v>
       </c>
       <c r="H19" s="39" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I19" s="39" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="69">
+      <c r="A20" s="68">
         <v>19</v>
       </c>
       <c r="B20" s="49"/>
@@ -3260,7 +3214,7 @@
       <c r="D20" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="78"/>
+      <c r="E20" s="89"/>
       <c r="F20" s="19" t="s">
         <v>86</v>
       </c>
@@ -3268,15 +3222,15 @@
         <v>80</v>
       </c>
       <c r="H20" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I20" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J20" s="42"/>
     </row>
     <row r="21" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="69">
+      <c r="A21" s="68">
         <v>20</v>
       </c>
       <c r="B21" s="49"/>
@@ -3286,7 +3240,7 @@
       <c r="D21" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="78"/>
+      <c r="E21" s="89"/>
       <c r="F21" s="19" t="s">
         <v>92</v>
       </c>
@@ -3294,15 +3248,15 @@
         <v>82</v>
       </c>
       <c r="H21" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I21" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J21" s="42"/>
     </row>
     <row r="22" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="70">
+      <c r="A22" s="69">
         <v>21</v>
       </c>
       <c r="B22" s="50"/>
@@ -3312,7 +3266,7 @@
       <c r="D22" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="80"/>
+      <c r="E22" s="91"/>
       <c r="F22" s="20" t="s">
         <v>91</v>
       </c>
@@ -3320,15 +3274,15 @@
         <v>81</v>
       </c>
       <c r="H22" s="43" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I22" s="43" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J22" s="44"/>
     </row>
     <row r="23" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="70">
+      <c r="A23" s="69">
         <v>22</v>
       </c>
       <c r="B23" s="48" t="s">
@@ -3340,8 +3294,8 @@
       <c r="D23" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="77" t="s">
-        <v>161</v>
+      <c r="E23" s="88" t="s">
+        <v>149</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>94</v>
@@ -3350,15 +3304,15 @@
         <v>95</v>
       </c>
       <c r="H23" s="39" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I23" s="39" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="70">
+      <c r="A24" s="69">
         <v>23</v>
       </c>
       <c r="B24" s="49"/>
@@ -3366,25 +3320,25 @@
         <v>40</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="E24" s="78"/>
+        <v>197</v>
+      </c>
+      <c r="E24" s="89"/>
       <c r="F24" s="19" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="H24" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I24" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J24" s="42"/>
     </row>
     <row r="25" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="70">
+      <c r="A25" s="69">
         <v>24</v>
       </c>
       <c r="B25" s="49"/>
@@ -3392,25 +3346,25 @@
         <v>40</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="E25" s="78"/>
+        <v>198</v>
+      </c>
+      <c r="E25" s="89"/>
       <c r="F25" s="19" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="H25" s="67" t="s">
-        <v>157</v>
-      </c>
-      <c r="I25" s="67" t="s">
-        <v>194</v>
+        <v>192</v>
+      </c>
+      <c r="H25" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="I25" s="66" t="s">
+        <v>182</v>
       </c>
       <c r="J25" s="42"/>
     </row>
     <row r="26" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="70">
+      <c r="A26" s="69">
         <v>25</v>
       </c>
       <c r="B26" s="49"/>
@@ -3418,25 +3372,25 @@
         <v>40</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="E26" s="78"/>
+        <v>199</v>
+      </c>
+      <c r="E26" s="89"/>
       <c r="F26" s="19" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="H26" s="67" t="s">
-        <v>157</v>
-      </c>
-      <c r="I26" s="67" t="s">
-        <v>194</v>
+        <v>196</v>
+      </c>
+      <c r="H26" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="I26" s="66" t="s">
+        <v>182</v>
       </c>
       <c r="J26" s="42"/>
     </row>
     <row r="27" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="70">
+      <c r="A27" s="69">
         <v>26</v>
       </c>
       <c r="B27" s="49"/>
@@ -3444,25 +3398,25 @@
         <v>40</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="E27" s="78"/>
+        <v>200</v>
+      </c>
+      <c r="E27" s="89"/>
       <c r="F27" s="19" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H27" s="67" t="s">
-        <v>157</v>
-      </c>
-      <c r="I27" s="67" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="H27" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="I27" s="66" t="s">
+        <v>182</v>
       </c>
       <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="69">
+      <c r="A28" s="68">
         <v>27</v>
       </c>
       <c r="B28" s="49"/>
@@ -3470,9 +3424,9 @@
         <v>40</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="E28" s="78"/>
+        <v>201</v>
+      </c>
+      <c r="E28" s="89"/>
       <c r="F28" s="19" t="s">
         <v>97</v>
       </c>
@@ -3480,15 +3434,15 @@
         <v>96</v>
       </c>
       <c r="H28" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I28" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="68">
+      <c r="A29" s="67">
         <v>28</v>
       </c>
       <c r="B29" s="49"/>
@@ -3496,21 +3450,21 @@
         <v>40</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="E29" s="78"/>
+        <v>202</v>
+      </c>
+      <c r="E29" s="89"/>
       <c r="F29" s="19" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
+        <v>204</v>
+      </c>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
       <c r="J29" s="42"/>
     </row>
     <row r="30" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="68">
+      <c r="A30" s="67">
         <v>29</v>
       </c>
       <c r="B30" s="49"/>
@@ -3518,25 +3472,25 @@
         <v>40</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="E30" s="78"/>
+        <v>208</v>
+      </c>
+      <c r="E30" s="89"/>
       <c r="F30" s="19" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="H30" s="71" t="s">
-        <v>223</v>
-      </c>
-      <c r="I30" s="71" t="s">
-        <v>194</v>
+        <v>210</v>
+      </c>
+      <c r="H30" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="I30" s="70" t="s">
+        <v>182</v>
       </c>
       <c r="J30" s="42"/>
     </row>
     <row r="31" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="68">
+      <c r="A31" s="67">
         <v>30</v>
       </c>
       <c r="B31" s="49"/>
@@ -3546,7 +3500,7 @@
       <c r="D31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="78"/>
+      <c r="E31" s="89"/>
       <c r="F31" s="19" t="s">
         <v>99</v>
       </c>
@@ -3554,15 +3508,15 @@
         <v>100</v>
       </c>
       <c r="H31" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I31" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J31" s="42"/>
     </row>
     <row r="32" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="68">
+      <c r="A32" s="67">
         <v>31</v>
       </c>
       <c r="B32" s="49"/>
@@ -3572,7 +3526,7 @@
       <c r="D32" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="78"/>
+      <c r="E32" s="89"/>
       <c r="F32" s="19" t="s">
         <v>102</v>
       </c>
@@ -3580,15 +3534,15 @@
         <v>103</v>
       </c>
       <c r="H32" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I32" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J32" s="42"/>
     </row>
     <row r="33" spans="1:10" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="68">
+      <c r="A33" s="67">
         <v>32</v>
       </c>
       <c r="B33" s="49"/>
@@ -3598,7 +3552,7 @@
       <c r="D33" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="78"/>
+      <c r="E33" s="89"/>
       <c r="F33" s="19" t="s">
         <v>105</v>
       </c>
@@ -3606,15 +3560,15 @@
         <v>106</v>
       </c>
       <c r="H33" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I33" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J33" s="42"/>
     </row>
     <row r="34" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="68">
+      <c r="A34" s="67">
         <v>33</v>
       </c>
       <c r="B34" s="49"/>
@@ -3624,7 +3578,7 @@
       <c r="D34" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="78"/>
+      <c r="E34" s="89"/>
       <c r="F34" s="19" t="s">
         <v>109</v>
       </c>
@@ -3632,15 +3586,15 @@
         <v>107</v>
       </c>
       <c r="H34" s="41" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="I34" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J34" s="42"/>
     </row>
     <row r="35" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="68">
+      <c r="A35" s="67">
         <v>34</v>
       </c>
       <c r="B35" s="49"/>
@@ -3648,25 +3602,25 @@
         <v>40</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E35" s="78"/>
+        <v>205</v>
+      </c>
+      <c r="E35" s="89"/>
       <c r="F35" s="19" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="G35" s="19" t="s">
         <v>108</v>
       </c>
       <c r="H35" s="41" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="I35" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J35" s="42"/>
     </row>
     <row r="36" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="68">
+      <c r="A36" s="67">
         <v>35</v>
       </c>
       <c r="B36" s="49"/>
@@ -3676,7 +3630,7 @@
       <c r="D36" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="78"/>
+      <c r="E36" s="89"/>
       <c r="F36" s="19" t="s">
         <v>111</v>
       </c>
@@ -3684,15 +3638,15 @@
         <v>116</v>
       </c>
       <c r="H36" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I36" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J36" s="42"/>
     </row>
     <row r="37" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="68">
+      <c r="A37" s="67">
         <v>36</v>
       </c>
       <c r="B37" s="50"/>
@@ -3702,7 +3656,7 @@
       <c r="D37" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="80"/>
+      <c r="E37" s="91"/>
       <c r="F37" s="20" t="s">
         <v>110</v>
       </c>
@@ -3710,15 +3664,15 @@
         <v>115</v>
       </c>
       <c r="H37" s="43" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I37" s="43" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J37" s="44"/>
     </row>
     <row r="38" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="68">
+      <c r="A38" s="67">
         <v>37</v>
       </c>
       <c r="B38" s="48" t="s">
@@ -3730,8 +3684,8 @@
       <c r="D38" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E38" s="77" t="s">
-        <v>162</v>
+      <c r="E38" s="88" t="s">
+        <v>150</v>
       </c>
       <c r="F38" s="18" t="s">
         <v>117</v>
@@ -3740,15 +3694,15 @@
         <v>118</v>
       </c>
       <c r="H38" s="39" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I38" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="68">
+      <c r="A39" s="67">
         <v>38</v>
       </c>
       <c r="B39" s="49"/>
@@ -3756,25 +3710,25 @@
         <v>40</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="E39" s="78"/>
+        <v>212</v>
+      </c>
+      <c r="E39" s="89"/>
       <c r="F39" s="19" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="H39" s="41" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I39" s="41" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J39" s="42"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="68">
+      <c r="A40" s="67">
         <v>39</v>
       </c>
       <c r="B40" s="50"/>
@@ -3784,7 +3738,7 @@
       <c r="D40" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E40" s="80"/>
+      <c r="E40" s="91"/>
       <c r="F40" s="20" t="s">
         <v>119</v>
       </c>
@@ -3792,15 +3746,15 @@
         <v>121</v>
       </c>
       <c r="H40" s="43" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I40" s="43" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J40" s="44"/>
     </row>
     <row r="41" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="68">
+      <c r="A41" s="67">
         <v>40</v>
       </c>
       <c r="B41" s="50"/>
@@ -3810,27 +3764,27 @@
       <c r="D41" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="73"/>
+      <c r="E41" s="72"/>
       <c r="F41" s="20" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="H41" s="72" t="s">
-        <v>157</v>
-      </c>
-      <c r="I41" s="72" t="s">
-        <v>194</v>
+      <c r="H41" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="I41" s="71" t="s">
+        <v>182</v>
       </c>
       <c r="J41" s="44"/>
     </row>
     <row r="42" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="82">
+      <c r="A42" s="76">
         <v>41</v>
       </c>
-      <c r="B42" s="83" t="s">
-        <v>236</v>
+      <c r="B42" s="77" t="s">
+        <v>224</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>40</v>
@@ -3838,159 +3792,159 @@
       <c r="D42" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="77" t="s">
-        <v>163</v>
+      <c r="E42" s="88" t="s">
+        <v>151</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G42" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="H42" s="74" t="s">
-        <v>157</v>
-      </c>
-      <c r="I42" s="74" t="s">
-        <v>194</v>
+      <c r="H42" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="I42" s="73" t="s">
+        <v>182</v>
       </c>
       <c r="J42" s="40"/>
     </row>
     <row r="43" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="84">
+      <c r="A43" s="78">
         <v>42</v>
       </c>
-      <c r="B43" s="85"/>
+      <c r="B43" s="79"/>
       <c r="C43" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E43" s="78"/>
+      <c r="E43" s="89"/>
       <c r="F43" s="19" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="H43" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="I43" s="75" t="s">
-        <v>194</v>
+        <v>215</v>
+      </c>
+      <c r="H43" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="I43" s="74" t="s">
+        <v>182</v>
       </c>
       <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="84">
+      <c r="A44" s="78">
         <v>43</v>
       </c>
-      <c r="B44" s="85"/>
+      <c r="B44" s="79"/>
       <c r="C44" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E44" s="78"/>
+      <c r="E44" s="89"/>
       <c r="F44" s="19" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G44" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="H44" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="I44" s="75" t="s">
-        <v>194</v>
+        <v>216</v>
+      </c>
+      <c r="H44" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="I44" s="74" t="s">
+        <v>182</v>
       </c>
       <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="84">
+      <c r="A45" s="78">
         <v>44</v>
       </c>
-      <c r="B45" s="85"/>
+      <c r="B45" s="79"/>
       <c r="C45" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="E45" s="78"/>
+        <v>221</v>
+      </c>
+      <c r="E45" s="89"/>
       <c r="F45" s="19" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="G45" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="H45" s="75" t="s">
-        <v>234</v>
-      </c>
-      <c r="I45" s="75" t="s">
-        <v>194</v>
+        <v>220</v>
+      </c>
+      <c r="H45" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="I45" s="74" t="s">
+        <v>182</v>
       </c>
       <c r="J45" s="42"/>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="84">
+      <c r="A46" s="78">
         <v>45</v>
       </c>
-      <c r="B46" s="85"/>
+      <c r="B46" s="79"/>
       <c r="C46" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E46" s="78"/>
+      <c r="E46" s="89"/>
       <c r="F46" s="19" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="G46" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H46" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="I46" s="75" t="s">
-        <v>194</v>
+      <c r="H46" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="I46" s="74" t="s">
+        <v>182</v>
       </c>
       <c r="J46" s="42"/>
     </row>
     <row r="47" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="86">
+      <c r="A47" s="80">
         <v>46</v>
       </c>
-      <c r="B47" s="87"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D47" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E47" s="80"/>
+      <c r="E47" s="91"/>
       <c r="F47" s="20" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H47" s="76" t="s">
-        <v>157</v>
-      </c>
-      <c r="I47" s="76" t="s">
-        <v>194</v>
+      <c r="H47" s="75" t="s">
+        <v>145</v>
+      </c>
+      <c r="I47" s="75" t="s">
+        <v>182</v>
       </c>
       <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="86">
+      <c r="A48" s="80">
         <v>47</v>
       </c>
-      <c r="B48" s="83" t="s">
-        <v>237</v>
+      <c r="B48" s="77" t="s">
+        <v>225</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>40</v>
@@ -3998,241 +3952,241 @@
       <c r="D48" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="77" t="s">
-        <v>238</v>
+      <c r="E48" s="88" t="s">
+        <v>226</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H48" s="74" t="s">
-        <v>157</v>
-      </c>
-      <c r="I48" s="74" t="s">
-        <v>194</v>
+        <v>129</v>
+      </c>
+      <c r="H48" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="I48" s="73" t="s">
+        <v>182</v>
       </c>
       <c r="J48" s="40"/>
     </row>
     <row r="49" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="94">
+      <c r="A49" s="87">
         <v>48</v>
       </c>
-      <c r="B49" s="85"/>
+      <c r="B49" s="79"/>
       <c r="C49" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E49" s="78"/>
+        <v>130</v>
+      </c>
+      <c r="E49" s="89"/>
       <c r="F49" s="19" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G49" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="H49" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="I49" s="75" t="s">
-        <v>240</v>
+        <v>131</v>
+      </c>
+      <c r="H49" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="I49" s="74" t="s">
+        <v>228</v>
       </c>
       <c r="J49" s="42" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="92">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="80">
         <v>49</v>
       </c>
-      <c r="B50" s="85"/>
+      <c r="B50" s="79"/>
       <c r="C50" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D50" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E50" s="89"/>
+      <c r="F50" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="G50" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="H50" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="I50" s="74" t="s">
+        <v>182</v>
+      </c>
+      <c r="J50" s="42"/>
+    </row>
+    <row r="51" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="80">
+        <v>50</v>
+      </c>
+      <c r="B51" s="79"/>
+      <c r="C51" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="E51" s="89"/>
+      <c r="F51" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="G51" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="H51" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="I51" s="74" t="s">
+        <v>182</v>
+      </c>
+      <c r="J51" s="42"/>
+    </row>
+    <row r="52" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="80">
+        <v>51</v>
+      </c>
+      <c r="B52" s="81"/>
+      <c r="C52" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E50" s="78"/>
-      <c r="F50" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="G50" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="H50" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="I50" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="J50" s="42"/>
-    </row>
-    <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="92">
-        <v>50</v>
-      </c>
-      <c r="B51" s="85"/>
-      <c r="C51" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E51" s="78"/>
-      <c r="F51" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="G51" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="H51" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="I51" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="J51" s="42"/>
-    </row>
-    <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="92">
-        <v>51</v>
-      </c>
-      <c r="B52" s="85"/>
-      <c r="C52" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E52" s="78"/>
-      <c r="F52" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="G52" s="19" t="s">
+      <c r="E52" s="91"/>
+      <c r="F52" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="G52" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="H52" s="75" t="s">
+        <v>145</v>
+      </c>
+      <c r="I52" s="75" t="s">
+        <v>182</v>
+      </c>
+      <c r="J52" s="44"/>
+    </row>
+    <row r="53" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="86">
+        <v>52</v>
+      </c>
+      <c r="B53" s="51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="H52" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="I52" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="J52" s="42"/>
-    </row>
-    <row r="53" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A53" s="92">
-        <v>52</v>
-      </c>
-      <c r="B53" s="85"/>
-      <c r="C53" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="E53" s="78"/>
-      <c r="F53" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G53" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="H53" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="I53" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="J53" s="42"/>
-    </row>
-    <row r="54" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="93">
+      <c r="G53" s="82" t="s">
+        <v>137</v>
+      </c>
+      <c r="H53" s="83" t="s">
+        <v>145</v>
+      </c>
+      <c r="I53" s="84" t="s">
+        <v>182</v>
+      </c>
+      <c r="J53" s="85"/>
+    </row>
+    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="87">
         <v>53</v>
       </c>
-      <c r="B54" s="87"/>
-      <c r="C54" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" s="80"/>
-      <c r="F54" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="G54" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="H54" s="76" t="s">
-        <v>157</v>
-      </c>
-      <c r="I54" s="76" t="s">
-        <v>194</v>
-      </c>
-      <c r="J54" s="44"/>
-    </row>
-    <row r="55" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="81">
+      <c r="B54" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="88" t="s">
+        <v>166</v>
+      </c>
+      <c r="F54" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="G54" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="H54" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="I54" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="J54" s="47"/>
+    </row>
+    <row r="55" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A55" s="87">
         <v>54</v>
       </c>
-      <c r="B55" s="51" t="s">
-        <v>197</v>
-      </c>
-      <c r="C55" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D55" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="G55" s="88" t="s">
-        <v>149</v>
-      </c>
-      <c r="H55" s="89" t="s">
-        <v>157</v>
-      </c>
-      <c r="I55" s="90" t="s">
-        <v>194</v>
-      </c>
-      <c r="J55" s="91"/>
-    </row>
-    <row r="56" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="64">
+      <c r="B55" s="53"/>
+      <c r="C55" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="E55" s="89"/>
+      <c r="F55" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="G55" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="H55" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="I55" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="J55" s="10"/>
+    </row>
+    <row r="56" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="87">
         <v>55</v>
       </c>
-      <c r="B56" s="52" t="s">
-        <v>170</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D56" s="36" t="s">
-        <v>165</v>
-      </c>
-      <c r="E56" s="77" t="s">
-        <v>178</v>
-      </c>
-      <c r="F56" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="G56" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="H56" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="I56" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="J56" s="47"/>
-    </row>
-    <row r="57" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="64">
+      <c r="B56" s="53"/>
+      <c r="C56" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="E56" s="89"/>
+      <c r="F56" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="G56" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="H56" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="I56" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="J56" s="10"/>
+    </row>
+    <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="87">
         <v>56</v>
       </c>
       <c r="B57" s="53"/>
@@ -4240,25 +4194,25 @@
         <v>40</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="E57" s="78"/>
+        <v>155</v>
+      </c>
+      <c r="E57" s="89"/>
       <c r="F57" s="34" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G57" s="34" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H57" s="35" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I57" s="35" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="J57" s="10"/>
     </row>
-    <row r="58" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="64">
+    <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="87">
         <v>57</v>
       </c>
       <c r="B58" s="53"/>
@@ -4266,25 +4220,25 @@
         <v>40</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="E58" s="78"/>
+        <v>157</v>
+      </c>
+      <c r="E58" s="89"/>
       <c r="F58" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="G58" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="H58" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="I58" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="G58" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="H58" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="I58" s="35" t="s">
-        <v>195</v>
-      </c>
       <c r="J58" s="10"/>
     </row>
-    <row r="59" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="64">
+    <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="87">
         <v>58</v>
       </c>
       <c r="B59" s="53"/>
@@ -4292,25 +4246,25 @@
         <v>40</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="E59" s="78"/>
+        <v>156</v>
+      </c>
+      <c r="E59" s="89"/>
       <c r="F59" s="34" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="G59" s="34" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H59" s="35" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I59" s="35" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="J59" s="10"/>
     </row>
-    <row r="60" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="64">
+    <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="87">
         <v>59</v>
       </c>
       <c r="B60" s="53"/>
@@ -4318,25 +4272,25 @@
         <v>40</v>
       </c>
       <c r="D60" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="E60" s="78"/>
+        <v>159</v>
+      </c>
+      <c r="E60" s="89"/>
       <c r="F60" s="34" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="G60" s="34" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H60" s="35" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I60" s="35" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="J60" s="10"/>
     </row>
-    <row r="61" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="64">
+    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="87">
         <v>60</v>
       </c>
       <c r="B61" s="53"/>
@@ -4344,25 +4298,25 @@
         <v>40</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="E61" s="78"/>
+        <v>160</v>
+      </c>
+      <c r="E61" s="89"/>
       <c r="F61" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="G61" s="34" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H61" s="35" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I61" s="35" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="J61" s="10"/>
     </row>
-    <row r="62" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="64">
+    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="87">
         <v>61</v>
       </c>
       <c r="B62" s="53"/>
@@ -4370,142 +4324,90 @@
         <v>40</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="E62" s="78"/>
+        <v>161</v>
+      </c>
+      <c r="E62" s="89"/>
       <c r="F62" s="34" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="G62" s="34" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="H62" s="35" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I62" s="35" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="J62" s="10"/>
     </row>
     <row r="63" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="64">
+      <c r="A63" s="87">
         <v>62</v>
       </c>
-      <c r="B63" s="53"/>
-      <c r="C63" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D63" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="E63" s="78"/>
-      <c r="F63" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="G63" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="H63" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="I63" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="J63" s="10"/>
-    </row>
-    <row r="64" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="64">
+      <c r="B63" s="55"/>
+      <c r="C63" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="E63" s="90"/>
+      <c r="F63" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="G63" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="H63" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="I63" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="J63" s="60"/>
+    </row>
+    <row r="64" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="87">
         <v>63</v>
       </c>
-      <c r="B64" s="53"/>
-      <c r="C64" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D64" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="E64" s="78"/>
-      <c r="F64" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="G64" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="H64" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="I64" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="J64" s="10"/>
-    </row>
-    <row r="65" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="64">
-        <v>64</v>
-      </c>
-      <c r="B65" s="55"/>
-      <c r="C65" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="D65" s="57" t="s">
-        <v>174</v>
-      </c>
-      <c r="E65" s="79"/>
-      <c r="F65" s="58" t="s">
-        <v>191</v>
-      </c>
-      <c r="G65" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="H65" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="I65" s="59" t="s">
-        <v>195</v>
-      </c>
-      <c r="J65" s="60"/>
-    </row>
-    <row r="66" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="64">
-        <v>65</v>
-      </c>
-      <c r="B66" s="61" t="s">
-        <v>175</v>
-      </c>
-      <c r="C66" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="D66" s="62" t="s">
-        <v>176</v>
-      </c>
-      <c r="E66" s="45"/>
-      <c r="F66" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="G66" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="H66" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="I66" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="J66" s="63"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="64"/>
+      <c r="B64" s="61" t="s">
+        <v>163</v>
+      </c>
+      <c r="C64" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="E64" s="45"/>
+      <c r="F64" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="G64" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="H64" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="I64" s="46" t="s">
+        <v>183</v>
+      </c>
+      <c r="J64" s="63"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="E56:E65"/>
+    <mergeCell ref="E54:E63"/>
     <mergeCell ref="E3:E8"/>
     <mergeCell ref="E9:E18"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="E23:E37"/>
     <mergeCell ref="E38:E40"/>
     <mergeCell ref="E42:E47"/>
-    <mergeCell ref="E48:E54"/>
+    <mergeCell ref="E48:E52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
refactor tests, add docs
</commit_message>
<xml_diff>
--- a/docs/check- сases.xlsx
+++ b/docs/check- сases.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="236">
   <si>
     <t>№</t>
   </si>
@@ -1014,9 +1014,6 @@
 6. Заявка создана</t>
   </si>
   <si>
-    <t>Заявка создается. Но ее не видно в списке.</t>
-  </si>
-  <si>
     <t>Фильтр: по дате</t>
   </si>
   <si>
@@ -1112,6 +1109,9 @@
   </si>
   <si>
     <t>Не возможно</t>
+  </si>
+  <si>
+    <t>Периодически возникает ошибка.</t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1778,67 +1778,61 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2671,8 +2665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,8 +2739,8 @@
       <c r="H2" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="I2" s="90" t="s">
-        <v>183</v>
+      <c r="I2" s="87" t="s">
+        <v>234</v>
       </c>
       <c r="J2" s="24"/>
     </row>
@@ -2763,7 +2757,7 @@
       <c r="D3" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="89" t="s">
         <v>148</v>
       </c>
       <c r="F3" s="18" t="s">
@@ -2791,7 +2785,7 @@
       <c r="D4" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="92"/>
+      <c r="E4" s="90"/>
       <c r="F4" s="19" t="s">
         <v>44</v>
       </c>
@@ -2801,11 +2795,11 @@
       <c r="H4" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="I4" s="89" t="s">
-        <v>182</v>
-      </c>
-      <c r="J4" s="90" t="s">
-        <v>228</v>
+      <c r="I4" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="J4" s="87" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2819,7 +2813,7 @@
       <c r="D5" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="92"/>
+      <c r="E5" s="90"/>
       <c r="F5" s="19" t="s">
         <v>45</v>
       </c>
@@ -2829,11 +2823,11 @@
       <c r="H5" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="I5" s="89" t="s">
-        <v>182</v>
-      </c>
-      <c r="J5" s="90" t="s">
-        <v>228</v>
+      <c r="I5" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="J5" s="87" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2847,7 +2841,7 @@
       <c r="D6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="92"/>
+      <c r="E6" s="90"/>
       <c r="F6" s="19" t="s">
         <v>46</v>
       </c>
@@ -2857,14 +2851,14 @@
       <c r="H6" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="I6" s="89" t="s">
-        <v>182</v>
-      </c>
-      <c r="J6" s="90" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="J6" s="87" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="67">
         <v>6</v>
       </c>
@@ -2875,7 +2869,7 @@
       <c r="D7" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="92"/>
+      <c r="E7" s="90"/>
       <c r="F7" s="19" t="s">
         <v>46</v>
       </c>
@@ -2885,11 +2879,11 @@
       <c r="H7" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="I7" s="89" t="s">
-        <v>182</v>
-      </c>
-      <c r="J7" s="90" t="s">
-        <v>228</v>
+      <c r="I7" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="J7" s="87" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2903,7 +2897,7 @@
       <c r="D8" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="94"/>
+      <c r="E8" s="92"/>
       <c r="F8" s="20" t="s">
         <v>49</v>
       </c>
@@ -2931,7 +2925,7 @@
       <c r="D9" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="E9" s="91" t="s">
+      <c r="E9" s="89" t="s">
         <v>146</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -2959,7 +2953,7 @@
       <c r="D10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="92"/>
+      <c r="E10" s="90"/>
       <c r="F10" s="15" t="s">
         <v>60</v>
       </c>
@@ -2985,7 +2979,7 @@
       <c r="D11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="92"/>
+      <c r="E11" s="90"/>
       <c r="F11" s="15" t="s">
         <v>61</v>
       </c>
@@ -3011,7 +3005,7 @@
       <c r="D12" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E12" s="92"/>
+      <c r="E12" s="90"/>
       <c r="F12" s="19" t="s">
         <v>62</v>
       </c>
@@ -3037,7 +3031,7 @@
       <c r="D13" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="E13" s="92"/>
+      <c r="E13" s="90"/>
       <c r="F13" s="19" t="s">
         <v>88</v>
       </c>
@@ -3063,7 +3057,7 @@
       <c r="D14" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="92"/>
+      <c r="E14" s="90"/>
       <c r="F14" s="19" t="s">
         <v>83</v>
       </c>
@@ -3089,7 +3083,7 @@
       <c r="D15" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="92"/>
+      <c r="E15" s="90"/>
       <c r="F15" s="19" t="s">
         <v>70</v>
       </c>
@@ -3115,7 +3109,7 @@
       <c r="D16" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="92"/>
+      <c r="E16" s="90"/>
       <c r="F16" s="19" t="s">
         <v>84</v>
       </c>
@@ -3141,7 +3135,7 @@
       <c r="D17" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="92"/>
+      <c r="E17" s="90"/>
       <c r="F17" s="19" t="s">
         <v>87</v>
       </c>
@@ -3167,7 +3161,7 @@
       <c r="D18" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="94"/>
+      <c r="E18" s="92"/>
       <c r="F18" s="20" t="s">
         <v>85</v>
       </c>
@@ -3195,7 +3189,7 @@
       <c r="D19" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="91" t="s">
+      <c r="E19" s="89" t="s">
         <v>146</v>
       </c>
       <c r="F19" s="18" t="s">
@@ -3223,7 +3217,7 @@
       <c r="D20" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="92"/>
+      <c r="E20" s="90"/>
       <c r="F20" s="19" t="s">
         <v>86</v>
       </c>
@@ -3249,7 +3243,7 @@
       <c r="D21" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="92"/>
+      <c r="E21" s="90"/>
       <c r="F21" s="19" t="s">
         <v>92</v>
       </c>
@@ -3275,7 +3269,7 @@
       <c r="D22" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="94"/>
+      <c r="E22" s="92"/>
       <c r="F22" s="20" t="s">
         <v>91</v>
       </c>
@@ -3303,7 +3297,7 @@
       <c r="D23" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="91" t="s">
+      <c r="E23" s="89" t="s">
         <v>149</v>
       </c>
       <c r="F23" s="18" t="s">
@@ -3331,7 +3325,7 @@
       <c r="D24" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="E24" s="92"/>
+      <c r="E24" s="90"/>
       <c r="F24" s="19" t="s">
         <v>189</v>
       </c>
@@ -3357,7 +3351,7 @@
       <c r="D25" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="E25" s="92"/>
+      <c r="E25" s="90"/>
       <c r="F25" s="19" t="s">
         <v>191</v>
       </c>
@@ -3383,7 +3377,7 @@
       <c r="D26" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="E26" s="92"/>
+      <c r="E26" s="90"/>
       <c r="F26" s="19" t="s">
         <v>193</v>
       </c>
@@ -3409,7 +3403,7 @@
       <c r="D27" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="E27" s="92"/>
+      <c r="E27" s="90"/>
       <c r="F27" s="19" t="s">
         <v>194</v>
       </c>
@@ -3435,7 +3429,7 @@
       <c r="D28" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="E28" s="92"/>
+      <c r="E28" s="90"/>
       <c r="F28" s="19" t="s">
         <v>97</v>
       </c>
@@ -3461,7 +3455,7 @@
       <c r="D29" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="E29" s="92"/>
+      <c r="E29" s="90"/>
       <c r="F29" s="19" t="s">
         <v>203</v>
       </c>
@@ -3483,22 +3477,20 @@
       <c r="D30" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="E30" s="92"/>
+      <c r="E30" s="90"/>
       <c r="F30" s="19" t="s">
         <v>209</v>
       </c>
       <c r="G30" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="H30" s="88" t="s">
-        <v>145</v>
-      </c>
-      <c r="I30" s="70" t="s">
-        <v>235</v>
-      </c>
-      <c r="J30" s="90" t="s">
-        <v>211</v>
-      </c>
+      <c r="H30" s="86" t="s">
+        <v>145</v>
+      </c>
+      <c r="I30" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="J30" s="42"/>
     </row>
     <row r="31" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="67">
@@ -3511,7 +3503,7 @@
       <c r="D31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="92"/>
+      <c r="E31" s="90"/>
       <c r="F31" s="19" t="s">
         <v>99</v>
       </c>
@@ -3537,7 +3529,7 @@
       <c r="D32" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="92"/>
+      <c r="E32" s="90"/>
       <c r="F32" s="19" t="s">
         <v>102</v>
       </c>
@@ -3563,7 +3555,7 @@
       <c r="D33" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="92"/>
+      <c r="E33" s="90"/>
       <c r="F33" s="19" t="s">
         <v>105</v>
       </c>
@@ -3589,20 +3581,22 @@
       <c r="D34" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="92"/>
+      <c r="E34" s="90"/>
       <c r="F34" s="19" t="s">
         <v>109</v>
       </c>
       <c r="G34" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="H34" s="90" t="s">
+      <c r="H34" s="87" t="s">
         <v>207</v>
       </c>
       <c r="I34" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="J34" s="42"/>
+      <c r="J34" s="87" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="67">
@@ -3615,20 +3609,22 @@
       <c r="D35" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="E35" s="92"/>
+      <c r="E35" s="90"/>
       <c r="F35" s="19" t="s">
         <v>206</v>
       </c>
       <c r="G35" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="H35" s="90" t="s">
+      <c r="H35" s="87" t="s">
         <v>207</v>
       </c>
       <c r="I35" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="J35" s="42"/>
+      <c r="J35" s="87" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="36" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="67">
@@ -3641,7 +3637,7 @@
       <c r="D36" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="92"/>
+      <c r="E36" s="90"/>
       <c r="F36" s="19" t="s">
         <v>111</v>
       </c>
@@ -3667,7 +3663,7 @@
       <c r="D37" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="94"/>
+      <c r="E37" s="92"/>
       <c r="F37" s="20" t="s">
         <v>110</v>
       </c>
@@ -3695,7 +3691,7 @@
       <c r="D38" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E38" s="91" t="s">
+      <c r="E38" s="89" t="s">
         <v>150</v>
       </c>
       <c r="F38" s="18" t="s">
@@ -3721,14 +3717,14 @@
         <v>40</v>
       </c>
       <c r="D39" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="E39" s="90"/>
+      <c r="F39" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="19" t="s">
+      <c r="G39" s="19" t="s">
         <v>213</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>214</v>
       </c>
       <c r="H39" s="41" t="s">
         <v>145</v>
@@ -3749,7 +3745,7 @@
       <c r="D40" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E40" s="94"/>
+      <c r="E40" s="92"/>
       <c r="F40" s="20" t="s">
         <v>119</v>
       </c>
@@ -3775,27 +3771,27 @@
       <c r="D41" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="72"/>
+      <c r="E41" s="71"/>
       <c r="F41" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="H41" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="I41" s="71" t="s">
+      <c r="H41" s="70" t="s">
+        <v>145</v>
+      </c>
+      <c r="I41" s="70" t="s">
         <v>182</v>
       </c>
       <c r="J41" s="44"/>
     </row>
     <row r="42" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="76">
+      <c r="A42" s="75">
         <v>41</v>
       </c>
-      <c r="B42" s="77" t="s">
-        <v>224</v>
+      <c r="B42" s="76" t="s">
+        <v>223</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>40</v>
@@ -3803,7 +3799,7 @@
       <c r="D42" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="91" t="s">
+      <c r="E42" s="89" t="s">
         <v>151</v>
       </c>
       <c r="F42" s="18" t="s">
@@ -3812,150 +3808,150 @@
       <c r="G42" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="H42" s="73" t="s">
-        <v>145</v>
-      </c>
-      <c r="I42" s="73" t="s">
+      <c r="H42" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="I42" s="72" t="s">
         <v>182</v>
       </c>
       <c r="J42" s="40"/>
     </row>
     <row r="43" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="78">
+      <c r="A43" s="77">
         <v>42</v>
       </c>
-      <c r="B43" s="79"/>
+      <c r="B43" s="78"/>
       <c r="C43" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E43" s="92"/>
+      <c r="E43" s="90"/>
       <c r="F43" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="H43" s="74" t="s">
-        <v>145</v>
-      </c>
-      <c r="I43" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="H43" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="I43" s="73" t="s">
         <v>182</v>
       </c>
       <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="78">
+      <c r="A44" s="77">
         <v>43</v>
       </c>
-      <c r="B44" s="79"/>
+      <c r="B44" s="78"/>
       <c r="C44" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E44" s="92"/>
+      <c r="E44" s="90"/>
       <c r="F44" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="H44" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="I44" s="73" t="s">
+        <v>182</v>
+      </c>
+      <c r="J44" s="42"/>
+    </row>
+    <row r="45" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="77">
+        <v>44</v>
+      </c>
+      <c r="B45" s="78"/>
+      <c r="C45" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="E45" s="90"/>
+      <c r="F45" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="G44" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="H44" s="74" t="s">
-        <v>145</v>
-      </c>
-      <c r="I44" s="74" t="s">
-        <v>182</v>
-      </c>
-      <c r="J44" s="42"/>
-    </row>
-    <row r="45" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="78">
-        <v>44</v>
-      </c>
-      <c r="B45" s="79"/>
-      <c r="C45" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" s="15" t="s">
+      <c r="G45" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="H45" s="87" t="s">
         <v>221</v>
       </c>
-      <c r="E45" s="92"/>
-      <c r="F45" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="H45" s="90" t="s">
-        <v>222</v>
-      </c>
-      <c r="I45" s="74" t="s">
+      <c r="I45" s="73" t="s">
         <v>182</v>
       </c>
       <c r="J45" s="42"/>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="78">
+      <c r="A46" s="77">
         <v>45</v>
       </c>
-      <c r="B46" s="79"/>
+      <c r="B46" s="78"/>
       <c r="C46" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E46" s="92"/>
+      <c r="E46" s="90"/>
       <c r="F46" s="19" t="s">
         <v>135</v>
       </c>
       <c r="G46" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H46" s="74" t="s">
-        <v>145</v>
-      </c>
-      <c r="I46" s="74" t="s">
+      <c r="H46" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="I46" s="73" t="s">
         <v>182</v>
       </c>
       <c r="J46" s="42"/>
     </row>
     <row r="47" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="80">
+      <c r="A47" s="79">
         <v>46</v>
       </c>
-      <c r="B47" s="81"/>
+      <c r="B47" s="80"/>
       <c r="C47" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D47" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E47" s="94"/>
+      <c r="E47" s="92"/>
       <c r="F47" s="20" t="s">
         <v>132</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H47" s="75" t="s">
-        <v>145</v>
-      </c>
-      <c r="I47" s="75" t="s">
+      <c r="H47" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="I47" s="74" t="s">
         <v>182</v>
       </c>
       <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="80">
+      <c r="A48" s="79">
         <v>47</v>
       </c>
-      <c r="B48" s="77" t="s">
-        <v>225</v>
+      <c r="B48" s="76" t="s">
+        <v>224</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>40</v>
@@ -3963,8 +3959,8 @@
       <c r="D48" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="91" t="s">
-        <v>226</v>
+      <c r="E48" s="89" t="s">
+        <v>225</v>
       </c>
       <c r="F48" s="18" t="s">
         <v>134</v>
@@ -3972,122 +3968,122 @@
       <c r="G48" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="H48" s="73" t="s">
-        <v>145</v>
-      </c>
-      <c r="I48" s="73" t="s">
+      <c r="H48" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="I48" s="72" t="s">
         <v>182</v>
       </c>
       <c r="J48" s="40"/>
     </row>
     <row r="49" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="80">
+      <c r="A49" s="79">
         <v>48</v>
       </c>
-      <c r="B49" s="79"/>
+      <c r="B49" s="78"/>
       <c r="C49" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="E49" s="92"/>
+      <c r="E49" s="90"/>
       <c r="F49" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G49" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="H49" s="74" t="s">
-        <v>145</v>
-      </c>
-      <c r="I49" s="87" t="s">
-        <v>182</v>
-      </c>
-      <c r="J49" s="90" t="s">
+      <c r="H49" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="I49" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="J49" s="87" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="79">
+        <v>49</v>
+      </c>
+      <c r="B50" s="78"/>
+      <c r="C50" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="15" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="80">
-        <v>49</v>
-      </c>
-      <c r="B50" s="79"/>
-      <c r="C50" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="15" t="s">
+      <c r="E50" s="90"/>
+      <c r="F50" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="19" t="s">
+      <c r="G50" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="G50" s="19" t="s">
+      <c r="H50" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="I50" s="73" t="s">
+        <v>182</v>
+      </c>
+      <c r="J50" s="42"/>
+    </row>
+    <row r="51" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="79">
+        <v>50</v>
+      </c>
+      <c r="B51" s="78"/>
+      <c r="C51" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="H50" s="74" t="s">
-        <v>145</v>
-      </c>
-      <c r="I50" s="74" t="s">
-        <v>182</v>
-      </c>
-      <c r="J50" s="42"/>
-    </row>
-    <row r="51" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="80">
-        <v>50</v>
-      </c>
-      <c r="B51" s="79"/>
-      <c r="C51" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D51" s="15" t="s">
+      <c r="E51" s="90"/>
+      <c r="F51" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="E51" s="92"/>
-      <c r="F51" s="19" t="s">
+      <c r="G51" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="G51" s="19" t="s">
-        <v>234</v>
-      </c>
-      <c r="H51" s="74" t="s">
-        <v>145</v>
-      </c>
-      <c r="I51" s="74" t="s">
+      <c r="H51" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="I51" s="73" t="s">
         <v>182</v>
       </c>
       <c r="J51" s="42"/>
     </row>
     <row r="52" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="80">
+      <c r="A52" s="79">
         <v>51</v>
       </c>
-      <c r="B52" s="81"/>
+      <c r="B52" s="80"/>
       <c r="C52" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D52" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E52" s="94"/>
+      <c r="E52" s="92"/>
       <c r="F52" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="H52" s="75" t="s">
-        <v>145</v>
-      </c>
-      <c r="I52" s="75" t="s">
+      <c r="H52" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="I52" s="74" t="s">
         <v>182</v>
       </c>
       <c r="J52" s="44"/>
     </row>
     <row r="53" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="80">
+      <c r="A53" s="79">
         <v>52</v>
       </c>
       <c r="B53" s="51" t="s">
@@ -4103,19 +4099,19 @@
       <c r="F53" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G53" s="82" t="s">
+      <c r="G53" s="81" t="s">
         <v>137</v>
       </c>
-      <c r="H53" s="83" t="s">
-        <v>145</v>
-      </c>
-      <c r="I53" s="84" t="s">
-        <v>182</v>
-      </c>
-      <c r="J53" s="85"/>
+      <c r="H53" s="82" t="s">
+        <v>145</v>
+      </c>
+      <c r="I53" s="83" t="s">
+        <v>182</v>
+      </c>
+      <c r="J53" s="84"/>
     </row>
     <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="86">
+      <c r="A54" s="85">
         <v>53</v>
       </c>
       <c r="B54" s="52" t="s">
@@ -4127,7 +4123,7 @@
       <c r="D54" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="E54" s="91" t="s">
+      <c r="E54" s="89" t="s">
         <v>166</v>
       </c>
       <c r="F54" s="37" t="s">
@@ -4139,13 +4135,13 @@
       <c r="H54" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="I54" s="90" t="s">
+      <c r="I54" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J54" s="47"/>
     </row>
     <row r="55" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A55" s="86">
+      <c r="A55" s="85">
         <v>54</v>
       </c>
       <c r="B55" s="53"/>
@@ -4155,7 +4151,7 @@
       <c r="D55" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="E55" s="92"/>
+      <c r="E55" s="90"/>
       <c r="F55" s="34" t="s">
         <v>170</v>
       </c>
@@ -4165,13 +4161,13 @@
       <c r="H55" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="I55" s="90" t="s">
+      <c r="I55" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J55" s="10"/>
     </row>
     <row r="56" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="86">
+      <c r="A56" s="85">
         <v>55</v>
       </c>
       <c r="B56" s="53"/>
@@ -4181,7 +4177,7 @@
       <c r="D56" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="E56" s="92"/>
+      <c r="E56" s="90"/>
       <c r="F56" s="34" t="s">
         <v>171</v>
       </c>
@@ -4191,13 +4187,13 @@
       <c r="H56" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="I56" s="90" t="s">
+      <c r="I56" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J56" s="10"/>
     </row>
     <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="86">
+      <c r="A57" s="85">
         <v>56</v>
       </c>
       <c r="B57" s="53"/>
@@ -4207,7 +4203,7 @@
       <c r="D57" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="E57" s="92"/>
+      <c r="E57" s="90"/>
       <c r="F57" s="34" t="s">
         <v>173</v>
       </c>
@@ -4217,13 +4213,13 @@
       <c r="H57" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="I57" s="90" t="s">
+      <c r="I57" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J57" s="10"/>
     </row>
     <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="86">
+      <c r="A58" s="85">
         <v>57</v>
       </c>
       <c r="B58" s="53"/>
@@ -4233,7 +4229,7 @@
       <c r="D58" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="E58" s="92"/>
+      <c r="E58" s="90"/>
       <c r="F58" s="34" t="s">
         <v>175</v>
       </c>
@@ -4243,13 +4239,13 @@
       <c r="H58" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="I58" s="90" t="s">
+      <c r="I58" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J58" s="10"/>
     </row>
     <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="86">
+      <c r="A59" s="85">
         <v>58</v>
       </c>
       <c r="B59" s="53"/>
@@ -4259,7 +4255,7 @@
       <c r="D59" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="E59" s="92"/>
+      <c r="E59" s="90"/>
       <c r="F59" s="34" t="s">
         <v>177</v>
       </c>
@@ -4269,13 +4265,13 @@
       <c r="H59" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="I59" s="90" t="s">
+      <c r="I59" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J59" s="10"/>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="86">
+      <c r="A60" s="85">
         <v>59</v>
       </c>
       <c r="B60" s="53"/>
@@ -4285,7 +4281,7 @@
       <c r="D60" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="E60" s="92"/>
+      <c r="E60" s="90"/>
       <c r="F60" s="34" t="s">
         <v>179</v>
       </c>
@@ -4295,13 +4291,13 @@
       <c r="H60" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="I60" s="90" t="s">
+      <c r="I60" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J60" s="10"/>
     </row>
     <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="86">
+      <c r="A61" s="85">
         <v>60</v>
       </c>
       <c r="B61" s="53"/>
@@ -4311,7 +4307,7 @@
       <c r="D61" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="E61" s="92"/>
+      <c r="E61" s="90"/>
       <c r="F61" s="34" t="s">
         <v>179</v>
       </c>
@@ -4321,13 +4317,13 @@
       <c r="H61" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="I61" s="90" t="s">
+      <c r="I61" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J61" s="10"/>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="86">
+      <c r="A62" s="85">
         <v>61</v>
       </c>
       <c r="B62" s="53"/>
@@ -4337,7 +4333,7 @@
       <c r="D62" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="E62" s="92"/>
+      <c r="E62" s="90"/>
       <c r="F62" s="34" t="s">
         <v>179</v>
       </c>
@@ -4347,13 +4343,13 @@
       <c r="H62" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="I62" s="90" t="s">
+      <c r="I62" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J62" s="10"/>
     </row>
     <row r="63" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="86">
+      <c r="A63" s="85">
         <v>62</v>
       </c>
       <c r="B63" s="55"/>
@@ -4363,7 +4359,7 @@
       <c r="D63" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="E63" s="93"/>
+      <c r="E63" s="91"/>
       <c r="F63" s="58" t="s">
         <v>179</v>
       </c>
@@ -4373,13 +4369,13 @@
       <c r="H63" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="I63" s="90" t="s">
+      <c r="I63" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J63" s="60"/>
     </row>
     <row r="64" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="86">
+      <c r="A64" s="85">
         <v>63</v>
       </c>
       <c r="B64" s="61" t="s">
@@ -4401,7 +4397,7 @@
       <c r="H64" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="I64" s="90" t="s">
+      <c r="I64" s="87" t="s">
         <v>183</v>
       </c>
       <c r="J64" s="63"/>

</xml_diff>